<commit_message>
merge updates from latest USDA commit
</commit_message>
<xml_diff>
--- a/dependencies/genotype_key.xlsx
+++ b/dependencies/genotype_key.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\project\diagnostic_virology_laboratory\MKillian\Analysis\results\influenza\HPAI\hpai_genotyping_blast\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF7486A1-5A20-4943-9078-E15723985112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A6269D-36F1-42AD-BA13-59A6B7F0910E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="981" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="189">
   <si>
     <t>Genotype</t>
   </si>
@@ -540,6 +540,66 @@
   </si>
   <si>
     <t>D1.2</t>
+  </si>
+  <si>
+    <t>D2.1</t>
+  </si>
+  <si>
+    <t>am25</t>
+  </si>
+  <si>
+    <t>am5N2</t>
+  </si>
+  <si>
+    <t>Minor95</t>
+  </si>
+  <si>
+    <t>am26</t>
+  </si>
+  <si>
+    <t>D1.3</t>
+  </si>
+  <si>
+    <t>Minor98</t>
+  </si>
+  <si>
+    <t>Minor99</t>
+  </si>
+  <si>
+    <t>Minor100</t>
+  </si>
+  <si>
+    <t>Minor101</t>
+  </si>
+  <si>
+    <t>am27</t>
+  </si>
+  <si>
+    <t>am6N2</t>
+  </si>
+  <si>
+    <t>am7N9</t>
+  </si>
+  <si>
+    <t>Minor97</t>
+  </si>
+  <si>
+    <t>Minor102</t>
+  </si>
+  <si>
+    <t>Minor103</t>
+  </si>
+  <si>
+    <t>Minor104</t>
+  </si>
+  <si>
+    <t>Minor105</t>
+  </si>
+  <si>
+    <t>Minor106</t>
+  </si>
+  <si>
+    <t>am8N5</t>
   </si>
 </sst>
 </file>
@@ -587,16 +647,16 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -626,7 +686,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -646,9 +706,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -954,16 +1013,18 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I109"/>
+  <dimension ref="A1:I122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="H117" sqref="H117"/>
+    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="L116" sqref="L116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="9" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -985,7 +1046,7 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -1136,8 +1197,8 @@
       <c r="H6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="2" t="s">
-        <v>18</v>
+      <c r="I6" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2000,7 +2061,7 @@
       <c r="F36" t="s">
         <v>33</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G36" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H36" t="s">
@@ -2029,7 +2090,7 @@
       <c r="F37" t="s">
         <v>23</v>
       </c>
-      <c r="G37" t="s">
+      <c r="G37" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H37" t="s">
@@ -2058,7 +2119,7 @@
       <c r="F38" t="s">
         <v>24</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G38" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H38" t="s">
@@ -2087,7 +2148,7 @@
       <c r="F39" t="s">
         <v>23</v>
       </c>
-      <c r="G39" t="s">
+      <c r="G39" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H39" t="s">
@@ -2116,7 +2177,7 @@
       <c r="F40" t="s">
         <v>24</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G40" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H40" t="s">
@@ -2145,7 +2206,7 @@
       <c r="F41" t="s">
         <v>23</v>
       </c>
-      <c r="G41" t="s">
+      <c r="G41" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H41" t="s">
@@ -2174,7 +2235,7 @@
       <c r="F42" t="s">
         <v>33</v>
       </c>
-      <c r="G42" t="s">
+      <c r="G42" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H42" t="s">
@@ -2203,7 +2264,7 @@
       <c r="F43" t="s">
         <v>33</v>
       </c>
-      <c r="G43" t="s">
+      <c r="G43" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H43" t="s">
@@ -2232,7 +2293,7 @@
       <c r="F44" t="s">
         <v>39</v>
       </c>
-      <c r="G44" t="s">
+      <c r="G44" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H44" t="s">
@@ -2261,7 +2322,7 @@
       <c r="F45" t="s">
         <v>23</v>
       </c>
-      <c r="G45" t="s">
+      <c r="G45" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H45" t="s">
@@ -2290,7 +2351,7 @@
       <c r="F46" t="s">
         <v>43</v>
       </c>
-      <c r="G46" t="s">
+      <c r="G46" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H46" t="s">
@@ -2319,7 +2380,7 @@
       <c r="F47" t="s">
         <v>24</v>
       </c>
-      <c r="G47" t="s">
+      <c r="G47" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H47" t="s">
@@ -2348,7 +2409,7 @@
       <c r="F48" t="s">
         <v>24</v>
       </c>
-      <c r="G48" t="s">
+      <c r="G48" s="8" t="s">
         <v>87</v>
       </c>
       <c r="H48" t="s">
@@ -2377,7 +2438,7 @@
       <c r="F49" t="s">
         <v>33</v>
       </c>
-      <c r="G49" t="s">
+      <c r="G49" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H49" t="s">
@@ -2406,7 +2467,7 @@
       <c r="F50" t="s">
         <v>33</v>
       </c>
-      <c r="G50" t="s">
+      <c r="G50" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H50" t="s">
@@ -2435,7 +2496,7 @@
       <c r="F51" t="s">
         <v>33</v>
       </c>
-      <c r="G51" t="s">
+      <c r="G51" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H51" t="s">
@@ -2464,7 +2525,7 @@
       <c r="F52" t="s">
         <v>23</v>
       </c>
-      <c r="G52" t="s">
+      <c r="G52" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H52" t="s">
@@ -2493,7 +2554,7 @@
       <c r="F53" t="s">
         <v>65</v>
       </c>
-      <c r="G53" t="s">
+      <c r="G53" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H53" t="s">
@@ -2522,7 +2583,7 @@
       <c r="F54" t="s">
         <v>33</v>
       </c>
-      <c r="G54" t="s">
+      <c r="G54" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H54" t="s">
@@ -2551,7 +2612,7 @@
       <c r="F55" t="s">
         <v>23</v>
       </c>
-      <c r="G55" t="s">
+      <c r="G55" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H55" t="s">
@@ -2580,7 +2641,7 @@
       <c r="F56" t="s">
         <v>90</v>
       </c>
-      <c r="G56" t="s">
+      <c r="G56" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H56" t="s">
@@ -2609,7 +2670,7 @@
       <c r="F57" t="s">
         <v>28</v>
       </c>
-      <c r="G57" t="s">
+      <c r="G57" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H57" t="s">
@@ -2638,7 +2699,7 @@
       <c r="F58" t="s">
         <v>33</v>
       </c>
-      <c r="G58" t="s">
+      <c r="G58" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H58" t="s">
@@ -2667,7 +2728,7 @@
       <c r="F59" t="s">
         <v>33</v>
       </c>
-      <c r="G59" t="s">
+      <c r="G59" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H59" t="s">
@@ -2696,7 +2757,7 @@
       <c r="F60" t="s">
         <v>24</v>
       </c>
-      <c r="G60" t="s">
+      <c r="G60" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H60" t="s">
@@ -2725,7 +2786,7 @@
       <c r="F61" t="s">
         <v>39</v>
       </c>
-      <c r="G61" t="s">
+      <c r="G61" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H61" t="s">
@@ -2754,7 +2815,7 @@
       <c r="F62" t="s">
         <v>33</v>
       </c>
-      <c r="G62" t="s">
+      <c r="G62" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H62" t="s">
@@ -2783,7 +2844,7 @@
       <c r="F63" t="s">
         <v>93</v>
       </c>
-      <c r="G63" t="s">
+      <c r="G63" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H63" t="s">
@@ -2812,7 +2873,7 @@
       <c r="F64" t="s">
         <v>10</v>
       </c>
-      <c r="G64" t="s">
+      <c r="G64" s="8" t="s">
         <v>12</v>
       </c>
       <c r="H64" t="s">
@@ -2841,7 +2902,7 @@
       <c r="F65" t="s">
         <v>39</v>
       </c>
-      <c r="G65" t="s">
+      <c r="G65" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H65" t="s">
@@ -2870,7 +2931,7 @@
       <c r="F66" t="s">
         <v>23</v>
       </c>
-      <c r="G66" t="s">
+      <c r="G66" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H66" t="s">
@@ -2899,7 +2960,7 @@
       <c r="F67" t="s">
         <v>23</v>
       </c>
-      <c r="G67" t="s">
+      <c r="G67" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H67" t="s">
@@ -2928,7 +2989,7 @@
       <c r="F68" t="s">
         <v>96</v>
       </c>
-      <c r="G68" t="s">
+      <c r="G68" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H68" t="s">
@@ -2957,7 +3018,7 @@
       <c r="F69" t="s">
         <v>23</v>
       </c>
-      <c r="G69" t="s">
+      <c r="G69" s="8" t="s">
         <v>116</v>
       </c>
       <c r="H69" t="s">
@@ -2986,7 +3047,7 @@
       <c r="F70" t="s">
         <v>95</v>
       </c>
-      <c r="G70" t="s">
+      <c r="G70" s="8" t="s">
         <v>12</v>
       </c>
       <c r="H70" t="s">
@@ -3015,7 +3076,7 @@
       <c r="F71" t="s">
         <v>90</v>
       </c>
-      <c r="G71" t="s">
+      <c r="G71" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H71" t="s">
@@ -3044,7 +3105,7 @@
       <c r="F72" t="s">
         <v>39</v>
       </c>
-      <c r="G72" t="s">
+      <c r="G72" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H72" t="s">
@@ -3073,7 +3134,7 @@
       <c r="F73" t="s">
         <v>10</v>
       </c>
-      <c r="G73" t="s">
+      <c r="G73" s="8" t="s">
         <v>12</v>
       </c>
       <c r="H73" t="s">
@@ -3102,7 +3163,7 @@
       <c r="F74" t="s">
         <v>33</v>
       </c>
-      <c r="G74" t="s">
+      <c r="G74" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H74" t="s">
@@ -3131,7 +3192,7 @@
       <c r="F75" t="s">
         <v>33</v>
       </c>
-      <c r="G75" t="s">
+      <c r="G75" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H75" t="s">
@@ -3160,7 +3221,7 @@
       <c r="F76" t="s">
         <v>24</v>
       </c>
-      <c r="G76" t="s">
+      <c r="G76" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H76" t="s">
@@ -3189,7 +3250,7 @@
       <c r="F77" t="s">
         <v>33</v>
       </c>
-      <c r="G77" t="s">
+      <c r="G77" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H77" t="s">
@@ -3218,7 +3279,7 @@
       <c r="F78" t="s">
         <v>33</v>
       </c>
-      <c r="G78" t="s">
+      <c r="G78" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H78" t="s">
@@ -3247,7 +3308,7 @@
       <c r="F79" t="s">
         <v>84</v>
       </c>
-      <c r="G79" t="s">
+      <c r="G79" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H79" t="s">
@@ -3276,7 +3337,7 @@
       <c r="F80" t="s">
         <v>10</v>
       </c>
-      <c r="G80" t="s">
+      <c r="G80" s="8" t="s">
         <v>12</v>
       </c>
       <c r="H80" t="s">
@@ -3305,7 +3366,7 @@
       <c r="F81" t="s">
         <v>96</v>
       </c>
-      <c r="G81" t="s">
+      <c r="G81" s="8" t="s">
         <v>12</v>
       </c>
       <c r="H81" t="s">
@@ -3334,7 +3395,7 @@
       <c r="F82" t="s">
         <v>95</v>
       </c>
-      <c r="G82" t="s">
+      <c r="G82" s="8" t="s">
         <v>12</v>
       </c>
       <c r="H82" t="s">
@@ -3363,7 +3424,7 @@
       <c r="F83" t="s">
         <v>33</v>
       </c>
-      <c r="G83" t="s">
+      <c r="G83" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H83" t="s">
@@ -3392,7 +3453,7 @@
       <c r="F84" t="s">
         <v>23</v>
       </c>
-      <c r="G84" t="s">
+      <c r="G84" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H84" t="s">
@@ -3421,7 +3482,7 @@
       <c r="F85" t="s">
         <v>93</v>
       </c>
-      <c r="G85" t="s">
+      <c r="G85" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H85" t="s">
@@ -3450,7 +3511,7 @@
       <c r="F86" t="s">
         <v>93</v>
       </c>
-      <c r="G86" t="s">
+      <c r="G86" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H86" t="s">
@@ -3479,7 +3540,7 @@
       <c r="F87" t="s">
         <v>33</v>
       </c>
-      <c r="G87" t="s">
+      <c r="G87" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H87" t="s">
@@ -3508,7 +3569,7 @@
       <c r="F88" t="s">
         <v>52</v>
       </c>
-      <c r="G88" t="s">
+      <c r="G88" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H88" t="s">
@@ -3537,7 +3598,7 @@
       <c r="F89" t="s">
         <v>33</v>
       </c>
-      <c r="G89" t="s">
+      <c r="G89" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H89" t="s">
@@ -3566,7 +3627,7 @@
       <c r="F90" t="s">
         <v>39</v>
       </c>
-      <c r="G90" t="s">
+      <c r="G90" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H90" t="s">
@@ -3595,7 +3656,7 @@
       <c r="F91" t="s">
         <v>10</v>
       </c>
-      <c r="G91" t="s">
+      <c r="G91" s="8" t="s">
         <v>12</v>
       </c>
       <c r="H91" t="s">
@@ -3624,7 +3685,7 @@
       <c r="F92" t="s">
         <v>84</v>
       </c>
-      <c r="G92" t="s">
+      <c r="G92" s="8" t="s">
         <v>12</v>
       </c>
       <c r="H92" t="s">
@@ -3653,7 +3714,7 @@
       <c r="F93" t="s">
         <v>52</v>
       </c>
-      <c r="G93" t="s">
+      <c r="G93" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H93" t="s">
@@ -3682,7 +3743,7 @@
       <c r="F94" t="s">
         <v>43</v>
       </c>
-      <c r="G94" t="s">
+      <c r="G94" s="8" t="s">
         <v>12</v>
       </c>
       <c r="H94" t="s">
@@ -3711,7 +3772,7 @@
       <c r="F95" t="s">
         <v>95</v>
       </c>
-      <c r="G95" t="s">
+      <c r="G95" s="8" t="s">
         <v>12</v>
       </c>
       <c r="H95" t="s">
@@ -3740,7 +3801,7 @@
       <c r="F96" t="s">
         <v>33</v>
       </c>
-      <c r="G96" t="s">
+      <c r="G96" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H96" t="s">
@@ -3769,7 +3830,7 @@
       <c r="F97" t="s">
         <v>57</v>
       </c>
-      <c r="G97" t="s">
+      <c r="G97" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H97" t="s">
@@ -3798,7 +3859,7 @@
       <c r="F98" t="s">
         <v>33</v>
       </c>
-      <c r="G98" t="s">
+      <c r="G98" s="8" t="s">
         <v>153</v>
       </c>
       <c r="H98" t="s">
@@ -3827,7 +3888,7 @@
       <c r="F99" t="s">
         <v>43</v>
       </c>
-      <c r="G99" t="s">
+      <c r="G99" s="8" t="s">
         <v>12</v>
       </c>
       <c r="H99" t="s">
@@ -3856,7 +3917,7 @@
       <c r="F100" t="s">
         <v>23</v>
       </c>
-      <c r="G100" t="s">
+      <c r="G100" s="8" t="s">
         <v>12</v>
       </c>
       <c r="H100" t="s">
@@ -3885,7 +3946,7 @@
       <c r="F101" t="s">
         <v>23</v>
       </c>
-      <c r="G101" t="s">
+      <c r="G101" s="8" t="s">
         <v>12</v>
       </c>
       <c r="H101" t="s">
@@ -3914,7 +3975,7 @@
       <c r="F102" t="s">
         <v>10</v>
       </c>
-      <c r="G102" t="s">
+      <c r="G102" s="8" t="s">
         <v>12</v>
       </c>
       <c r="H102" t="s">
@@ -3943,7 +4004,7 @@
       <c r="F103" t="s">
         <v>43</v>
       </c>
-      <c r="G103" t="s">
+      <c r="G103" s="8" t="s">
         <v>12</v>
       </c>
       <c r="H103" t="s">
@@ -3972,7 +4033,7 @@
       <c r="F104" t="s">
         <v>24</v>
       </c>
-      <c r="G104" t="s">
+      <c r="G104" s="8" t="s">
         <v>12</v>
       </c>
       <c r="H104" t="s">
@@ -4001,7 +4062,7 @@
       <c r="F105" t="s">
         <v>95</v>
       </c>
-      <c r="G105" t="s">
+      <c r="G105" s="8" t="s">
         <v>12</v>
       </c>
       <c r="H105" t="s">
@@ -4030,7 +4091,7 @@
       <c r="F106" t="s">
         <v>10</v>
       </c>
-      <c r="G106" t="s">
+      <c r="G106" s="8" t="s">
         <v>12</v>
       </c>
       <c r="H106" t="s">
@@ -4041,7 +4102,7 @@
       </c>
     </row>
     <row r="107" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="6" t="s">
+      <c r="A107" s="1" t="s">
         <v>164</v>
       </c>
       <c r="B107" t="s">
@@ -4059,7 +4120,7 @@
       <c r="F107" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="G107" t="s">
+      <c r="G107" s="8" t="s">
         <v>12</v>
       </c>
       <c r="H107" t="s">
@@ -4070,7 +4131,7 @@
       </c>
     </row>
     <row r="108" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="6" t="s">
+      <c r="A108" s="1" t="s">
         <v>165</v>
       </c>
       <c r="B108" s="5" t="s">
@@ -4098,11 +4159,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A109" s="6" t="s">
+    <row r="109" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B109" s="7" t="s">
+      <c r="B109" s="6" t="s">
         <v>166</v>
       </c>
       <c r="C109" t="s">
@@ -4114,16 +4175,393 @@
       <c r="E109" t="s">
         <v>14</v>
       </c>
-      <c r="F109" s="7" t="s">
+      <c r="F109" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G109" s="7" t="s">
+      <c r="G109" s="6" t="s">
         <v>167</v>
       </c>
       <c r="H109" t="s">
         <v>14</v>
       </c>
       <c r="I109" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B110" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="C110" t="s">
+        <v>14</v>
+      </c>
+      <c r="D110" t="s">
+        <v>39</v>
+      </c>
+      <c r="E110" t="s">
+        <v>14</v>
+      </c>
+      <c r="F110" t="s">
+        <v>23</v>
+      </c>
+      <c r="G110" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="H110" t="s">
+        <v>14</v>
+      </c>
+      <c r="I110" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B111" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="C111" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="D111" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E111" t="s">
+        <v>14</v>
+      </c>
+      <c r="F111" t="s">
+        <v>14</v>
+      </c>
+      <c r="G111" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H111" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I111" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B112" t="s">
+        <v>166</v>
+      </c>
+      <c r="C112" t="s">
+        <v>14</v>
+      </c>
+      <c r="D112" t="s">
+        <v>39</v>
+      </c>
+      <c r="E112" t="s">
+        <v>14</v>
+      </c>
+      <c r="F112" t="s">
+        <v>36</v>
+      </c>
+      <c r="G112" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H112" t="s">
+        <v>14</v>
+      </c>
+      <c r="I112" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B113" t="s">
+        <v>32</v>
+      </c>
+      <c r="C113" t="s">
+        <v>14</v>
+      </c>
+      <c r="D113" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="E113" t="s">
+        <v>14</v>
+      </c>
+      <c r="F113" t="s">
+        <v>119</v>
+      </c>
+      <c r="G113" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="H113" t="s">
+        <v>14</v>
+      </c>
+      <c r="I113" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B114" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="C114" t="s">
+        <v>14</v>
+      </c>
+      <c r="D114" t="s">
+        <v>39</v>
+      </c>
+      <c r="E114" t="s">
+        <v>14</v>
+      </c>
+      <c r="F114" t="s">
+        <v>36</v>
+      </c>
+      <c r="G114" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="H114" t="s">
+        <v>14</v>
+      </c>
+      <c r="I114" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B115" t="s">
+        <v>41</v>
+      </c>
+      <c r="C115" t="s">
+        <v>14</v>
+      </c>
+      <c r="D115" t="s">
+        <v>39</v>
+      </c>
+      <c r="E115" t="s">
+        <v>14</v>
+      </c>
+      <c r="F115" t="s">
+        <v>36</v>
+      </c>
+      <c r="G115" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="H115" t="s">
+        <v>14</v>
+      </c>
+      <c r="I115" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B116" t="s">
+        <v>166</v>
+      </c>
+      <c r="C116" t="s">
+        <v>14</v>
+      </c>
+      <c r="D116" t="s">
+        <v>39</v>
+      </c>
+      <c r="E116" t="s">
+        <v>14</v>
+      </c>
+      <c r="F116" t="s">
+        <v>84</v>
+      </c>
+      <c r="G116" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="H116" t="s">
+        <v>14</v>
+      </c>
+      <c r="I116" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B117" t="s">
+        <v>166</v>
+      </c>
+      <c r="C117" t="s">
+        <v>14</v>
+      </c>
+      <c r="D117" t="s">
+        <v>39</v>
+      </c>
+      <c r="E117" t="s">
+        <v>14</v>
+      </c>
+      <c r="F117" t="s">
+        <v>14</v>
+      </c>
+      <c r="G117" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="H117" t="s">
+        <v>14</v>
+      </c>
+      <c r="I117" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B118" t="s">
+        <v>23</v>
+      </c>
+      <c r="C118" t="s">
+        <v>14</v>
+      </c>
+      <c r="D118" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="E118" t="s">
+        <v>14</v>
+      </c>
+      <c r="F118" t="s">
+        <v>36</v>
+      </c>
+      <c r="G118" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="H118" t="s">
+        <v>14</v>
+      </c>
+      <c r="I118" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B119" t="s">
+        <v>179</v>
+      </c>
+      <c r="C119" t="s">
+        <v>14</v>
+      </c>
+      <c r="D119" t="s">
+        <v>14</v>
+      </c>
+      <c r="E119" t="s">
+        <v>14</v>
+      </c>
+      <c r="F119" t="s">
+        <v>14</v>
+      </c>
+      <c r="G119" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H119" t="s">
+        <v>14</v>
+      </c>
+      <c r="I119" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B120" t="s">
+        <v>23</v>
+      </c>
+      <c r="C120" t="s">
+        <v>14</v>
+      </c>
+      <c r="D120" t="s">
+        <v>39</v>
+      </c>
+      <c r="E120" t="s">
+        <v>14</v>
+      </c>
+      <c r="F120" t="s">
+        <v>36</v>
+      </c>
+      <c r="G120" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="H120" t="s">
+        <v>14</v>
+      </c>
+      <c r="I120" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B121" t="s">
+        <v>45</v>
+      </c>
+      <c r="C121" t="s">
+        <v>14</v>
+      </c>
+      <c r="D121" t="s">
+        <v>39</v>
+      </c>
+      <c r="E121" t="s">
+        <v>14</v>
+      </c>
+      <c r="F121" t="s">
+        <v>36</v>
+      </c>
+      <c r="G121" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H121" t="s">
+        <v>14</v>
+      </c>
+      <c r="I121" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B122" t="s">
+        <v>14</v>
+      </c>
+      <c r="C122" t="s">
+        <v>14</v>
+      </c>
+      <c r="D122" t="s">
+        <v>14</v>
+      </c>
+      <c r="E122" t="s">
+        <v>14</v>
+      </c>
+      <c r="F122" t="s">
+        <v>84</v>
+      </c>
+      <c r="G122" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H122" t="s">
+        <v>14</v>
+      </c>
+      <c r="I122" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>